<commit_message>
Checking in multiple loans for SBO
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDriver/TestSBO/ActivityData_FEB3.xlsx
+++ b/src/test/resources/TestDriver/TestSBO/ActivityData_FEB3.xlsx
@@ -5,19 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ssctechnologiesinc-my.sharepoint.com/personal/rafay_ahmed_sscinc_com/Documents/Desktop/Pers/SBO/All_Trigger/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arahmed\OneDrive - SS&amp;C Technologies, Inc\Desktop\Pers\SBO\All_Trigger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_E568B71B9998C0C804BC02B4C20AFA907A1AE5C3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A290342-B153-4643-9ECC-FDE57327BA8A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE5C66D-8893-437C-8AFD-1FE0EFD36FD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TransactionActivity" sheetId="3" r:id="rId1"/>
     <sheet name="GLRule" sheetId="7" state="hidden" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="8" state="hidden" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -38,10 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="40">
-  <si>
-    <t>IDHJ-EGNY</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="42">
   <si>
     <t>Postingdate</t>
   </si>
@@ -158,6 +155,15 @@
   </si>
   <si>
     <t>Def Rev</t>
+  </si>
+  <si>
+    <t>LOAN1</t>
+  </si>
+  <si>
+    <t>LOAN2</t>
+  </si>
+  <si>
+    <t>LOAN3</t>
   </si>
 </sst>
 </file>
@@ -510,10 +516,10 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -527,22 +533,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -553,15 +559,55 @@
         <v>44595</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2" s="7">
         <v>210</v>
       </c>
       <c r="F2" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>44595</v>
+      </c>
+      <c r="B3" s="5">
+        <v>44595</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="7">
+        <v>310</v>
+      </c>
+      <c r="F3" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>44595</v>
+      </c>
+      <c r="B4" s="5">
+        <v>44595</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="7">
+        <v>410</v>
+      </c>
+      <c r="F4" s="6">
         <v>1</v>
       </c>
     </row>
@@ -592,27 +638,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="C2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="D2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="F2" s="8" t="s">
         <v>13</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -624,16 +670,16 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -645,16 +691,16 @@
         <v>2</v>
       </c>
       <c r="C4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>16</v>
-      </c>
       <c r="E4" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -666,16 +712,16 @@
         <v>3</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="10" t="s">
         <v>20</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -687,16 +733,16 @@
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -708,16 +754,16 @@
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -729,16 +775,16 @@
         <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -750,16 +796,16 @@
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -771,16 +817,16 @@
         <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -792,16 +838,16 @@
         <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -813,16 +859,16 @@
         <v>10</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -834,16 +880,16 @@
         <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -855,16 +901,16 @@
         <v>12</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -897,45 +943,45 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>25</v>
       </c>
       <c r="I1" s="8"/>
     </row>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="1">
+        <v>100</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="1">
-        <v>100</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="H2" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E3" s="1">
         <v>-100</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
@@ -951,25 +997,25 @@
       </c>
       <c r="E5" s="10"/>
       <c r="G5" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C6" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10">
         <v>-100</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
@@ -977,7 +1023,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D8" s="10">
         <v>200</v>
@@ -985,15 +1031,15 @@
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
       <c r="G8" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C9" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="10">
@@ -1001,30 +1047,30 @@
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="J10" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="K10" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="K10" s="10" t="s">
+      <c r="L10" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="L10" s="10" t="s">
+      <c r="M10" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="M10" s="10" t="s">
+      <c r="N10" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="N10" s="10" t="s">
+      <c r="O10" s="10" t="s">
         <v>34</v>
-      </c>
-      <c r="O10" s="10" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
@@ -1032,16 +1078,16 @@
         <v>3</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D11" s="1">
         <v>200</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M11" s="1">
         <v>100</v>
@@ -1052,7 +1098,7 @@
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E12" s="1">
         <v>-200</v>
@@ -1062,7 +1108,7 @@
         <v>Revenue</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J12" s="10">
         <f>O11</f>
@@ -1100,16 +1146,16 @@
         <v>3</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D14" s="1">
         <v>1200</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K14" s="10">
         <f t="shared" ref="K14:K22" si="0">N13</f>
@@ -1125,7 +1171,7 @@
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E15" s="1">
         <v>-1200</v>
@@ -1135,7 +1181,7 @@
         <v>Def Revenue</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K15" s="10">
         <f t="shared" si="0"/>
@@ -1169,16 +1215,16 @@
         <v>3</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D17" s="1">
         <v>100</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K17" s="10">
         <f t="shared" si="0"/>
@@ -1195,7 +1241,7 @@
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E18" s="1">
         <v>-100</v>
@@ -1205,7 +1251,7 @@
         <v>Revenue</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K18" s="10">
         <f t="shared" si="0"/>
@@ -1250,16 +1296,16 @@
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K21" s="10">
         <f t="shared" si="0"/>

</xml_diff>